<commit_message>
modified:   admin/citas.xlsx 	modified:   admin/controllers/sistema.php 	modified:   admin/ws/doctor.php
</commit_message>
<xml_diff>
--- a/admin/citas.xlsx
+++ b/admin/citas.xlsx
@@ -15,11 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
-  <si>
-    <t>This is my first Excel</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -369,9 +365,7 @@
       <c r="A1"/>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
+      <c r="A2"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>